<commit_message>
atualizei a sprint backlog e o product
</commit_message>
<xml_diff>
--- a/documentacao/requisitos/Requisitos.xlsx
+++ b/documentacao/requisitos/Requisitos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PI\grupo9-ads\Requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PI\grupo9-ads\documentacao\requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E46CBA-F0E6-47DB-B2A4-259D6057B932}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionais" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t>Descrição</t>
   </si>
@@ -182,12 +181,18 @@
   </si>
   <si>
     <t>Ter api que controla a temperatura e umidade das geladeiras</t>
+  </si>
+  <si>
+    <t>RF13</t>
+  </si>
+  <si>
+    <t>Deve ter um site institucional explicando as funcionalidades da solução</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -293,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,6 +333,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -670,11 +681,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,14 +876,20 @@
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
@@ -952,7 +969,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:C33 C2:C23" xr:uid="{D1C3E77C-7649-4BAF-936B-1CC1A2AF9EA0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:C33 C2:C23">
       <formula1>$F$1:$F$2</formula1>
     </dataValidation>
   </dataValidations>
@@ -962,7 +979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -1108,7 +1125,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C10" xr:uid="{04C0F63B-1635-442D-94B6-997633ED140B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C10">
       <formula1>$E$1:$E$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
atualizada planilha de requisitos, funcional e não funcional. Adicionando planilha de cadastro (interno)
</commit_message>
<xml_diff>
--- a/documentacao/requisitos/Requisitos.xlsx
+++ b/documentacao/requisitos/Requisitos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitória Cristina\Desktop\grupo9-ads\documentacao\requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teodoro\Desktop\grupo9-ads\documentacao\requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E8D9EE-B9FC-4933-97DC-866177DB84AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983A6EE9-93F7-4419-9688-764008674042}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t>Descrição</t>
   </si>
@@ -206,13 +206,25 @@
   </si>
   <si>
     <t>Deve armazenar temperatura e umidade em um banco de dados</t>
+  </si>
+  <si>
+    <t>RF13</t>
+  </si>
+  <si>
+    <t>Ter planliha interna para cadastro de futuros clientes</t>
+  </si>
+  <si>
+    <t>RNF14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Os dados de cadastro de novos clientes deverá ser feito internamente </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +249,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -289,7 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -332,24 +352,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Ênfase1" xfId="1" builtinId="31"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -806,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFA6BF8-9A3E-4444-9492-F7A2EFB0701C}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,16 +873,16 @@
     <col min="3" max="3" width="17.5703125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -840,7 +895,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -851,7 +906,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -862,7 +917,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -873,7 +928,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -884,7 +939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -895,7 +950,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -906,7 +961,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -917,7 +972,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -928,7 +983,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -939,7 +994,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -949,8 +1004,9 @@
       <c r="C12" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -961,7 +1017,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -972,12 +1028,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="14"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="9"/>
       <c r="C16" s="14"/>
@@ -1021,13 +1083,13 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="C22:C27 C3:C19">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"desejavel"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"importante"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"essencial"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1037,7 +1099,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1045,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B3856E-DD8D-4670-BE01-99A966618F94}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,11 +1119,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1100,7 +1162,7 @@
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1111,7 +1173,7 @@
       <c r="A6" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1122,7 +1184,7 @@
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -1133,7 +1195,7 @@
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1144,7 +1206,7 @@
       <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -1155,7 +1217,7 @@
       <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1218,7 +1280,15 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+      <c r="A16" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -1228,8 +1298,19 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C10">
+    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
+      <formula>"desejável"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="23" operator="equal">
+      <formula>"importante"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
+      <formula>"essencial"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C12">
     <cfRule type="cellIs" dxfId="14" priority="19" operator="equal">
-      <formula>"desejável"</formula>
+      <formula>"desejavel"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
       <formula>"importante"</formula>
@@ -1238,7 +1319,7 @@
       <formula>"essencial"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C12">
+  <conditionalFormatting sqref="C13">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
       <formula>"desejavel"</formula>
     </cfRule>
@@ -1249,31 +1330,31 @@
       <formula>"essencial"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
-      <formula>"desejavel"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+  <conditionalFormatting sqref="C14">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"desejável"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"importante"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
-      <formula>"essencial"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
-      <formula>"desejável"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
-      <formula>"importante"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>"essencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"desejável"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"importante"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"essencial"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"desejável"</formula>
+      <formula>"desejavel"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"importante"</formula>
@@ -1286,7 +1367,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C10 C14:C15" xr:uid="{C6F5360B-DB5B-4CA4-B863-AD2A5CE9B45D}">
       <formula1>$E$1:$E$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C15" xr:uid="{5C488CB7-DA63-4D28-85F8-3F7BD819D4E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C16" xr:uid="{5C488CB7-DA63-4D28-85F8-3F7BD819D4E8}">
       <formula1>$F$1:$F$2</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>